<commit_message>
Atualização Planilha 31/07/2024 (DRONE)
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linco\Documents\Público\Pessoal\Estudos\streamlit\Lcl Finanças\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1837A6B-5DE0-44F3-BAB2-A08725E03426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671FD9A9-28BD-4BB3-A565-D85CF542A5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{5DBD2B94-81C0-4838-B20C-D5AC3920124A}"/>
+    <workbookView xWindow="4500" yWindow="840" windowWidth="21600" windowHeight="11385" xr2:uid="{5DBD2B94-81C0-4838-B20C-D5AC3920124A}"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="46">
   <si>
     <t>Projeto</t>
   </si>
@@ -161,13 +161,16 @@
     <t>pc</t>
   </si>
   <si>
-    <t>localizar NF</t>
-  </si>
-  <si>
     <t>CIMENTO</t>
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>providenciar NF</t>
+  </si>
+  <si>
+    <t>DRONE DJI AIR 2S FLY MORE COMBO</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B4E5DA-CF18-4382-AFE0-B2EB8B93E94F}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1175,7 @@
         <v>100</v>
       </c>
       <c r="I3" s="6">
-        <f t="shared" ref="I3:I21" si="0">G3*H3</f>
+        <f t="shared" ref="I3:I22" si="0">G3*H3</f>
         <v>100</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1242,7 +1245,7 @@
         <v>950</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1275,7 +1278,7 @@
         <v>1000</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1759,10 +1762,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" t="s">
         <v>43</v>
-      </c>
-      <c r="F21" t="s">
-        <v>44</v>
       </c>
       <c r="G21" s="4">
         <v>100</v>
@@ -1775,7 +1778,38 @@
         <v>3100</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45499</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f>"000638"</f>
+        <v>000638</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" s="6">
+        <v>9790</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="0"/>
+        <v>9790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização Planilha - 02/08/2024
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linco\Documents\Público\Pessoal\Estudos\streamlit\Lcl Finanças\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671FD9A9-28BD-4BB3-A565-D85CF542A5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26479C01-D5B9-42B4-8244-DA070D250326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="840" windowWidth="21600" windowHeight="11385" xr2:uid="{5DBD2B94-81C0-4838-B20C-D5AC3920124A}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{5DBD2B94-81C0-4838-B20C-D5AC3920124A}"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="50">
   <si>
     <t>Projeto</t>
   </si>
@@ -161,9 +161,6 @@
     <t>pc</t>
   </si>
   <si>
-    <t>CIMENTO</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
@@ -171,6 +168,21 @@
   </si>
   <si>
     <t>DRONE DJI AIR 2S FLY MORE COMBO</t>
+  </si>
+  <si>
+    <t>CIMENTO CP II F 32 ENSACADO 50KG - MOC</t>
+  </si>
+  <si>
+    <t>000.002.109</t>
+  </si>
+  <si>
+    <t>ART - EXECUÇÃO (CARAMURU)</t>
+  </si>
+  <si>
+    <t>RACHINHA</t>
+  </si>
+  <si>
+    <t>vb</t>
   </si>
 </sst>
 </file>
@@ -670,7 +682,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -688,6 +700,21 @@
     </xf>
     <xf numFmtId="43" fontId="13" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1065,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B4E5DA-CF18-4382-AFE0-B2EB8B93E94F}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1272,7 @@
         <v>950</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1278,7 +1305,7 @@
         <v>1000</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1748,37 +1775,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="9">
         <v>45503</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="4">
+      <c r="G21" s="10">
         <v>100</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="12">
         <v>31</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="12">
         <f t="shared" si="0"/>
         <v>3100</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>44</v>
+      <c r="J21" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1796,7 +1823,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
         <v>30</v>
@@ -1810,6 +1837,108 @@
       <c r="I22" s="6">
         <f t="shared" si="0"/>
         <v>9790</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45505</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6">
+        <v>10000</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" ref="I23" si="3">G23*H23</f>
+        <v>10000</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45505</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6">
+        <v>262.55</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" ref="I24:I25" si="4">G24*H24</f>
+        <v>262.55</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45506</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1070</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="4"/>
+        <v>1070</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>